<commit_message>
saving notes on 206
</commit_message>
<xml_diff>
--- a/0 NeetCode/206. Reverse Linked List/Whiteboards/Solution.xlsx
+++ b/0 NeetCode/206. Reverse Linked List/Whiteboards/Solution.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Portalz\Desktop\Small Projects\LeetCode\0 template\Whiteboards\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Portalz\Desktop\Small Projects\LeetCode\0 NeetCode\206. Reverse Linked List\Whiteboards\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{713DE802-9519-4608-B352-D1C1ED0E8E9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E6FCC22-AFE6-410F-8918-4128D67B8717}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{756CC0B2-6BE7-4EF6-9EEE-182F71A93026}"/>
   </bookViews>
@@ -34,6 +34,38 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="9">
+  <si>
+    <t>&gt;</t>
+  </si>
+  <si>
+    <t>&lt;</t>
+  </si>
+  <si>
+    <t>H</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t>prev=H</t>
+  </si>
+  <si>
+    <t>current=head.next</t>
+  </si>
+  <si>
+    <t>head=current.next</t>
+  </si>
+  <si>
+    <t>current.next=prev</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
@@ -45,12 +77,24 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -65,9 +109,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -384,17 +434,289 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79CF585D-CE06-44D4-80AA-070156E711E0}">
-  <dimension ref="A1"/>
+  <dimension ref="H6:AE27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="AD11" sqref="AD11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.7109375" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="16384" width="4.7109375" style="1"/>
   </cols>
-  <sheetData/>
+  <sheetData>
+    <row r="6" spans="8:31" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="T6" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="8:31" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H7" s="1">
+        <v>1</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="J7" s="1">
+        <v>2</v>
+      </c>
+      <c r="K7" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="L7" s="1">
+        <v>3</v>
+      </c>
+      <c r="M7" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="N7" s="1">
+        <v>4</v>
+      </c>
+      <c r="O7" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="P7" s="1">
+        <v>5</v>
+      </c>
+      <c r="W7" s="1">
+        <v>1</v>
+      </c>
+      <c r="X7" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="Y7" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="8:31" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H8" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="W8" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="X8" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y8" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="AA8" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="8:31" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AE10" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="8:31" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AE11" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="8:31" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AE12" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="8:31" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H13" s="1">
+        <v>1</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="J13" s="1">
+        <v>2</v>
+      </c>
+      <c r="K13" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="L13" s="1">
+        <v>3</v>
+      </c>
+      <c r="M13" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="N13" s="1">
+        <v>4</v>
+      </c>
+      <c r="O13" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="P13" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="8:31" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H14" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="I14" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="L14" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="8:31" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H16" s="1">
+        <v>1</v>
+      </c>
+      <c r="I16" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="J16" s="1">
+        <v>2</v>
+      </c>
+      <c r="K16" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="L16" s="1">
+        <v>3</v>
+      </c>
+      <c r="M16" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="N16" s="1">
+        <v>4</v>
+      </c>
+      <c r="O16" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="P16" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="8:30" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H17" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="I17" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="J17" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="L17" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="8:30" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J18" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="8:30" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H20" s="1">
+        <v>1</v>
+      </c>
+      <c r="I20" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="J20" s="1">
+        <v>2</v>
+      </c>
+      <c r="K20" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="L20" s="1">
+        <v>3</v>
+      </c>
+      <c r="M20" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="N20" s="1">
+        <v>4</v>
+      </c>
+      <c r="O20" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="P20" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="8:30" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I21" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="J21" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="L21" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="8:30" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L22" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="8:30" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H24" s="1">
+        <v>1</v>
+      </c>
+      <c r="I24" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="J24" s="1">
+        <v>2</v>
+      </c>
+      <c r="K24" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="L24" s="1">
+        <v>3</v>
+      </c>
+      <c r="M24" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="N24" s="1">
+        <v>4</v>
+      </c>
+      <c r="O24" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="P24" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" spans="8:30" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I25" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="J25" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="K25" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="L25" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="N25" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="8:30" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AD27" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>